<commit_message>
Enabled firefox to execute test
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/SeleniumGrid.xlsx
+++ b/src/test/resources/test-data/SeleniumGrid.xlsx
@@ -1,25 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Work/tdcs_framework/virtuoso-skeleton/src/test/resources/test-data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="12440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11310" windowHeight="3075" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Input Values" sheetId="1" r:id="rId1"/>
     <sheet name="Expected Results" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Configuration.Browser.Type</t>
   </si>
@@ -52,9 +45,6 @@
   </si>
   <si>
     <t>ANY</t>
-  </si>
-  <si>
-    <t>Chrome</t>
   </si>
 </sst>
 </file>
@@ -149,7 +139,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -184,7 +174,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -361,7 +351,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -372,23 +362,23 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -396,7 +386,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -404,7 +394,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -412,7 +402,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -433,9 +423,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>

</xml_diff>